<commit_message>
deposito parte1 e 2 19/08/2025
</commit_message>
<xml_diff>
--- a/tk_caixaEletronico/Base_Dados.xlsx
+++ b/tk_caixaEletronico/Base_Dados.xlsx
@@ -523,7 +523,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1074,6 +1074,62 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>567</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Clevison</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>678.234.987-89</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Depósito</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>19/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>567</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Clevison</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>678.234.987-89</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Saque</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>700</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>19/08/2025</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>